<commit_message>
Added a basic filter_by_keywords() refactor that simply returns a string. Functionality still unaffected
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bokwoon/Documents/SIMS-scraping/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858FDFF0-38E0-B247-837A-203D8C3534D1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="237">
   <si>
     <t>ASO255</t>
   </si>
@@ -28,7 +23,7 @@
     <t>Petrographic Examination of Aggregates for Concrete</t>
   </si>
   <si>
-    <t>BS EN 932-3                       </t>
+    <t xml:space="preserve">BS EN 932-3                       </t>
   </si>
   <si>
     <t>T00938</t>
@@ -40,7 +35,7 @@
     <t>ASO210</t>
   </si>
   <si>
-    <t>BS 812-104                                                                         </t>
+    <t xml:space="preserve">BS 812-104                                                                         </t>
   </si>
   <si>
     <t>ASO078</t>
@@ -736,19 +731,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -764,27 +760,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+  <cellXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -1072,1108 +1056,1109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="3" width="50.83203125" style="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
         <v>83</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
         <v>87</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>94</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
         <v>97</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>98</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
         <v>99</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
         <v>101</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
         <v>105</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
         <v>107</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
         <v>109</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>110</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
         <v>112</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>113</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
         <v>115</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>113</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>113</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
         <v>119</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>120</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
         <v>121</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
         <v>124</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>122</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
         <v>126</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>122</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
         <v>128</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" t="s">
         <v>129</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
         <v>131</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>132</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
         <v>134</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>135</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
         <v>136</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>137</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
         <v>139</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" t="s">
         <v>137</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
         <v>141</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" t="s">
         <v>142</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
         <v>144</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" t="s">
         <v>142</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
         <v>146</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" t="s">
         <v>147</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
         <v>149</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" t="s">
         <v>150</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
         <v>152</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" t="s">
         <v>153</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
         <v>155</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" t="s">
         <v>153</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
         <v>157</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" t="s">
         <v>158</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
         <v>160</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" t="s">
         <v>161</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
         <v>163</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" t="s">
         <v>164</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
         <v>166</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" t="s">
         <v>167</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
         <v>169</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" t="s">
         <v>170</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
         <v>172</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" t="s">
         <v>170</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
         <v>174</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" t="s">
         <v>175</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
         <v>177</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" t="s">
         <v>178</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
         <v>180</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" t="s">
         <v>181</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
         <v>182</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" t="s">
         <v>183</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
         <v>184</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" t="s">
         <v>185</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
         <v>187</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" t="s">
         <v>185</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
         <v>189</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" t="s">
         <v>185</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
         <v>191</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" t="s">
         <v>192</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
         <v>194</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" t="s">
         <v>195</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
         <v>197</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" t="s">
         <v>198</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
         <v>200</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" t="s">
         <v>195</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
         <v>202</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" t="s">
         <v>198</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
         <v>204</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" t="s">
         <v>195</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
         <v>204</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" t="s">
         <v>195</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
         <v>207</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" t="s">
         <v>208</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
         <v>210</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" t="s">
         <v>211</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
         <v>213</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" t="s">
         <v>214</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
         <v>216</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" t="s">
         <v>217</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
         <v>219</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" t="s">
         <v>220</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
         <v>222</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" t="s">
         <v>223</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
         <v>225</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" t="s">
         <v>226</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
         <v>228</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" t="s">
         <v>229</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
         <v>231</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" t="s">
         <v>232</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
         <v>234</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" t="s">
         <v>235</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" t="s">
         <v>236</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Keyword based matching works (whew what a lot of work)
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SinTemp.IT\Documents\SIMS-scraping\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="237">
   <si>
     <t>ASO255</t>
   </si>
@@ -23,7 +27,7 @@
     <t>Petrographic Examination of Aggregates for Concrete</t>
   </si>
   <si>
-    <t xml:space="preserve">BS EN 932-3                       </t>
+    <t>BS EN 932-3                       </t>
   </si>
   <si>
     <t>T00938</t>
@@ -35,7 +39,7 @@
     <t>ASO210</t>
   </si>
   <si>
-    <t xml:space="preserve">BS 812-104                                                                         </t>
+    <t>BS 812-104                                                                         </t>
   </si>
   <si>
     <t>ASO078</t>
@@ -167,7 +171,7 @@
     <t>BS 812-2</t>
   </si>
   <si>
-    <t>Searched for "SS 73" with 12 hits but no item matches "Bulk Density (Compacted and Uncompacted) &amp; Void" exactly</t>
+    <t>T00994:Bulk Density (Compacted and Loose) &amp; Voids</t>
   </si>
   <si>
     <t>SS 73</t>
@@ -227,7 +231,7 @@
     <t>ASTM C40</t>
   </si>
   <si>
-    <t>Searched for "SS 73" with 12 hits but no item matches "Organic Impurites" exactly</t>
+    <t>T00196:Organic Impurities</t>
   </si>
   <si>
     <t>T00988</t>
@@ -251,7 +255,7 @@
     <t>BS EN 933-7</t>
   </si>
   <si>
-    <t>Searched for "SS 73" with 12 hits but no item matches "Flakiness Index" exactly</t>
+    <t>T00996:Elongation Index</t>
   </si>
   <si>
     <t>Flakiness Index</t>
@@ -353,7 +357,7 @@
     <t>ASTM C88</t>
   </si>
   <si>
-    <t>Searched for "BS 812" with 32 hits but no item matches "Magnesium Sulfate Soundness" exactly</t>
+    <t>ASO209:Soundness in Magnesium Sulfate</t>
   </si>
   <si>
     <t>Magnesium Sulfate Soundness</t>
@@ -731,20 +735,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -760,15 +763,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1056,1109 +1071,1109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="50.6328125" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
+    <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
+    <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
+    <row r="54" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
+    <row r="66" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
-      <c r="A69" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
+    <row r="70" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
+    <row r="72" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
+    <row r="76" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
+    <row r="77" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
+    <row r="78" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
+    <row r="79" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
-      <c r="A84" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
-      <c r="A85" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
-      <c r="A86" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
-      <c r="A89" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
-      <c r="A90" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
-      <c r="A93" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
-      <c r="A94" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
-      <c r="A95" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
-      <c r="A96" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
-      <c r="A97" t="s">
+    <row r="97" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
-      <c r="A99" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="1" t="s">
         <v>236</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored filter_by_keywords() into filter_and_verify_multiple_entries(). Couldn't justify why I had to create so many functions just to serve obtan_id().
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -1074,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
It is done. The identification module is done.
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SinTemp.IT\Documents\SIMS-scraping\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="238">
   <si>
     <t>ASO255</t>
   </si>
@@ -23,7 +27,7 @@
     <t>Petrographic Examination of Aggregates for Concrete</t>
   </si>
   <si>
-    <t xml:space="preserve">BS EN 932-3                       </t>
+    <t>BS EN 932-3                       </t>
   </si>
   <si>
     <t>T00938</t>
@@ -35,7 +39,7 @@
     <t>ASO210</t>
   </si>
   <si>
-    <t xml:space="preserve">BS 812-104                                                                         </t>
+    <t>BS 812-104                                                                         </t>
   </si>
   <si>
     <t>ASO078</t>
@@ -62,7 +66,7 @@
     <t xml:space="preserve">SS 73                         </t>
   </si>
   <si>
-    <t>ASO165</t>
+    <t>ASO003</t>
   </si>
   <si>
     <t>ASTM C136</t>
@@ -110,13 +114,13 @@
     <t>SS 73 Cl 14 Method C</t>
   </si>
   <si>
-    <t>T00491:Particle Size Distribution|  ASO166:Particle Size Distribution (Sieve Analysis)|  T00067:Silt &amp; Clay Content</t>
+    <t>T00491| Particle Size Distribution  ~  ASO166| Particle Size Distribution (Sieve Analysis)  ~  T00067| Silt &amp; Clay Content</t>
   </si>
   <si>
     <t>Fines Content (Clay, Silt and Dust)</t>
   </si>
   <si>
-    <t>ASO149:Materials finer than 75  µm</t>
+    <t>ASO149| Materials finer than 75  µm</t>
   </si>
   <si>
     <t>ASTM C117</t>
@@ -158,7 +162,7 @@
     <t>BS EN 1097-3</t>
   </si>
   <si>
-    <t>ASO119:Bulk Density (Compacted and Loose) &amp; Voids</t>
+    <t>ASO119| Bulk Density (Compacted and Loose) &amp; Voids| BS 812-2</t>
   </si>
   <si>
     <t>Bulk Density (Compacted and Uncompacted) &amp; Void</t>
@@ -167,13 +171,13 @@
     <t>BS 812-2</t>
   </si>
   <si>
-    <t>T00994:Bulk Density (Compacted and Loose) &amp; Voids</t>
+    <t>T00994| Bulk Density (Compacted and Loose) &amp; Voids| SS 73</t>
   </si>
   <si>
     <t>SS 73</t>
   </si>
   <si>
-    <t>ASO258:Specific gravity &amp; Water Absorption|  ASO177:Thermal and weathering properties</t>
+    <t>ASO051| Density &amp; Water Absorption  ~  ASO082| Density &amp; Water Absorption</t>
   </si>
   <si>
     <t>Particle Density &amp; Water Absorption</t>
@@ -182,10 +186,13 @@
     <t>BS EN 1097-6</t>
   </si>
   <si>
+    <t>ASO156| Particle density  &amp; water absorption  ~  ASO157| Particle density  &amp; water absorption  ~  ASO155| Particle density &amp; water absorption</t>
+  </si>
+  <si>
     <t>T00197</t>
   </si>
   <si>
-    <t>ASO169:Particle Density &amp; Water Absorption|  T01201:Water Absorption of Coarse Aggregate</t>
+    <t>ASO169| Particle Density &amp; Water Absorption  ~  T01201| Water Absorption of Coarse Aggregate</t>
   </si>
   <si>
     <t>Relative Density (Specific Gravity) &amp; Water Absorption</t>
@@ -194,7 +201,7 @@
     <t>ASTM C127</t>
   </si>
   <si>
-    <t>ASO170:Particle Density &amp; Water Absorption|  T01202:Water Absorption of Fine Aggregate</t>
+    <t>ASO170| Particle Density &amp; Water Absorption  ~  T01202| Water Absorption of Fine Aggregate</t>
   </si>
   <si>
     <t>ASTM C128 Gravimetric Method</t>
@@ -218,7 +225,7 @@
     <t>T00987</t>
   </si>
   <si>
-    <t>CSR061:Organic Impurities|  ASO191:Organic Impurities in Sand</t>
+    <t>CSR061| Organic Impurities| ASTM C40  ~  CHM043| Organic impurities in sand| ASTM C40: 2004  ~  ASO191| Organic Impurities in Sand| ASTM C40</t>
   </si>
   <si>
     <t>Organic Impurites</t>
@@ -227,7 +234,7 @@
     <t>ASTM C40</t>
   </si>
   <si>
-    <t>T00196:Organic Impurities</t>
+    <t>T00196| Organic Impurities| SS 73</t>
   </si>
   <si>
     <t>T00988</t>
@@ -245,13 +252,13 @@
     <t>BS 812-106</t>
   </si>
   <si>
-    <t>ASO213:Shell Content|  ASO257:Shell Content</t>
+    <t>ASO213| Shell Content  ~  ASO257| Shell Content</t>
   </si>
   <si>
     <t>BS EN 933-7</t>
   </si>
   <si>
-    <t>T00996:Elongation Index</t>
+    <t>T00132</t>
   </si>
   <si>
     <t>Flakiness Index</t>
@@ -260,7 +267,7 @@
     <t>SS 73 Part 5.1</t>
   </si>
   <si>
-    <t>ASO053:Flakiness Index|  ASO118:Flakiness Index</t>
+    <t>ASO053| Flakiness Index  ~  ASO118| Flakiness Index</t>
   </si>
   <si>
     <t>BS EN 933-3</t>
@@ -314,7 +321,7 @@
     <t>10% Fines Value</t>
   </si>
   <si>
-    <t>ASO174:Ten percent fines value</t>
+    <t>ASO174| Ten percent fines value</t>
   </si>
   <si>
     <t>BS 812-111</t>
@@ -353,7 +360,7 @@
     <t>ASTM C88</t>
   </si>
   <si>
-    <t>ASO209:Soundness in Magnesium Sulfate</t>
+    <t>ASO209| Soundness in Magnesium Sulfate| BS 812 Part 121</t>
   </si>
   <si>
     <t>Magnesium Sulfate Soundness</t>
@@ -368,7 +375,7 @@
     <t>BS EN 1367-2</t>
   </si>
   <si>
-    <t>Searched for "SS 73" with 12 hits but no item matches "Magnesium Sulfate Soundness" exactly</t>
+    <t>T00131| Acid Soluble Sulphate Content| SS 73 Pt 18  ~  T00989| Total Sulfate Content by Acid Extraction| SS 73: Part 18 Cl 6  ~  T00999| Water-soluble Sulfates| SS 73: Part 18 Cl 5</t>
   </si>
   <si>
     <t>SS 73 Part 21</t>
@@ -434,7 +441,7 @@
     <t>BS EN 933-8</t>
   </si>
   <si>
-    <t>ASO168:Sand Equivalent Value</t>
+    <t>ASO168| Sand Equivalent Value</t>
   </si>
   <si>
     <t>ASTM D2419</t>
@@ -455,7 +462,7 @@
     <t>SS 544: Part 2 Annex B</t>
   </si>
   <si>
-    <t>Searched for "BS EN 1744-1" with 7 hits but no item matches "Organic Contaminators by Mortar Method" exactly</t>
+    <t>T01088| Lightweight Organic Contaminator| BS EN 1744-1 Cl 14.2</t>
   </si>
   <si>
     <t>Organic Contaminators by Mortar Method</t>
@@ -539,7 +546,7 @@
     <t>BS 812-114</t>
   </si>
   <si>
-    <t>CHE016:Lightweight Particle Analysis|  ASO143:Lightweight pieces</t>
+    <t>CHE016| Lightweight Particle Analysis  ~  ASO143| Lightweight pieces</t>
   </si>
   <si>
     <t>Lightweight Particles in Aggregate</t>
@@ -638,7 +645,7 @@
     <t>BS EN 1744-1 Cl 10.2</t>
   </si>
   <si>
-    <t>T00129</t>
+    <t>CCH002</t>
   </si>
   <si>
     <t>Acid Soluble Sulfates</t>
@@ -701,7 +708,7 @@
     <t>BS EN 1744-1 Cl 15.2</t>
   </si>
   <si>
-    <t>Searched for "BS EN 1744-1" with 7 hits but no item matches "Loss on Ignition" exactly</t>
+    <t>ASO091</t>
   </si>
   <si>
     <t>Loss on Ignition</t>
@@ -731,20 +738,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -760,15 +766,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1056,1109 +1074,1109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="50.6328125" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="24" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C26" t="s">
+      <c r="B26" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
+      <c r="C26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
+      <c r="B27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B28" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C28" t="s">
+      <c r="B28" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
+      <c r="C28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
+      <c r="B29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="31" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C31" t="s">
+      <c r="B31" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
+      <c r="C31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C33" t="s">
+      <c r="B33" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+      <c r="C33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B34" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+      <c r="B34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+      <c r="B35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B36" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C36" t="s">
+      <c r="B36" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+      <c r="C36" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B37" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
+      <c r="B37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B38" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
+      <c r="B38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B39" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C39" t="s">
+      <c r="B39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B40" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
+      <c r="C40" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B41" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C41" t="s">
+      <c r="B41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B42" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
+      <c r="C42" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B43" t="s">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C43" t="s">
+      <c r="B43" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B44" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
+      <c r="C44" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B45" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C45" t="s">
+      <c r="B45" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B46" t="s">
-        <v>98</v>
-      </c>
-      <c r="C46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
+      <c r="C46" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B47" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C47" t="s">
+      <c r="B47" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B48" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
+      <c r="C48" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B49" t="s">
-        <v>102</v>
-      </c>
-      <c r="C49" t="s">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
+      <c r="B49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B50" t="s">
-        <v>102</v>
-      </c>
-      <c r="C50" t="s">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
+      <c r="B50" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B51" t="s">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C51" t="s">
+      <c r="B51" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
+      <c r="C51" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B52" t="s">
+    </row>
+    <row r="52" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C52" t="s">
+      <c r="B52" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
+      <c r="C52" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B53" t="s">
-        <v>113</v>
-      </c>
-      <c r="C53" t="s">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
+      <c r="B53" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B54" t="s">
-        <v>113</v>
-      </c>
-      <c r="C54" t="s">
+    </row>
+    <row r="54" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
+      <c r="B54" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B55" t="s">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C55" t="s">
+      <c r="B55" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>121</v>
-      </c>
-      <c r="B56" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C56" t="s">
+      <c r="B56" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
+      <c r="C56" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B57" t="s">
-        <v>122</v>
-      </c>
-      <c r="C57" t="s">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
+      <c r="B57" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B58" t="s">
-        <v>122</v>
-      </c>
-      <c r="C58" t="s">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
+      <c r="B58" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B59" t="s">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C59" t="s">
+      <c r="B59" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
+      <c r="C59" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B60" t="s">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C60" t="s">
+      <c r="B60" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
+      <c r="C60" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B61" t="s">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C61" t="s">
+      <c r="B61" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>136</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C62" t="s">
+      <c r="B62" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
+      <c r="C62" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B63" t="s">
-        <v>137</v>
-      </c>
-      <c r="C63" t="s">
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
+      <c r="B63" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B64" t="s">
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C64" t="s">
+      <c r="B64" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
+      <c r="C64" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B65" t="s">
-        <v>142</v>
-      </c>
-      <c r="C65" t="s">
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
+      <c r="B65" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B66" t="s">
+    </row>
+    <row r="66" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C66" t="s">
+      <c r="B66" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
+      <c r="C66" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B67" t="s">
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C67" t="s">
+      <c r="B67" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
+      <c r="C67" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B68" t="s">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C68" t="s">
+      <c r="B68" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" t="s">
+      <c r="C68" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B69" t="s">
-        <v>153</v>
-      </c>
-      <c r="C69" t="s">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
+      <c r="B69" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B70" t="s">
+    </row>
+    <row r="70" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C70" t="s">
+      <c r="B70" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
+      <c r="C70" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B71" t="s">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C71" t="s">
+      <c r="B71" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
+      <c r="C71" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B72" t="s">
+    </row>
+    <row r="72" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C72" t="s">
+      <c r="B72" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
+      <c r="C72" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B73" t="s">
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C73" t="s">
+      <c r="B73" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
+      <c r="C73" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B74" t="s">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C74" t="s">
+      <c r="B74" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
+      <c r="C74" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B75" t="s">
-        <v>170</v>
-      </c>
-      <c r="C75" t="s">
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
+      <c r="B75" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B76" t="s">
+    </row>
+    <row r="76" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C76" t="s">
+      <c r="B76" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
+      <c r="C76" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B77" t="s">
+    </row>
+    <row r="77" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C77" t="s">
+      <c r="B77" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
+      <c r="C77" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B78" t="s">
+    </row>
+    <row r="78" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C78" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
+      <c r="B78" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C78" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C79" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
+      <c r="B79" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C79" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C80" t="s">
+      <c r="B80" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
+      <c r="C80" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B81" t="s">
-        <v>185</v>
-      </c>
-      <c r="C81" t="s">
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
+      <c r="B81" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B82" t="s">
-        <v>185</v>
-      </c>
-      <c r="C82" t="s">
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
+      <c r="B82" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B83" t="s">
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C83" t="s">
+      <c r="B83" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" t="s">
+      <c r="C83" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B84" t="s">
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C84" t="s">
+      <c r="B84" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" t="s">
+      <c r="C84" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B85" t="s">
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C85" t="s">
+      <c r="B85" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" t="s">
+      <c r="C85" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B86" t="s">
-        <v>195</v>
-      </c>
-      <c r="C86" t="s">
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
+      <c r="B86" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B87" t="s">
-        <v>198</v>
-      </c>
-      <c r="C87" t="s">
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
+      <c r="B87" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B88" t="s">
-        <v>195</v>
-      </c>
-      <c r="C88" t="s">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" t="s">
-        <v>204</v>
-      </c>
-      <c r="B89" t="s">
-        <v>195</v>
-      </c>
-      <c r="C89" t="s">
+      <c r="B88" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
-      <c r="A90" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B90" t="s">
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C90" t="s">
+      <c r="B90" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
+      <c r="C90" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B91" t="s">
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C91" t="s">
+      <c r="B91" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
+      <c r="C91" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B92" t="s">
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C92" t="s">
+      <c r="B92" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" t="s">
+      <c r="C92" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B93" t="s">
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C93" t="s">
+      <c r="B93" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" t="s">
+      <c r="C93" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B94" t="s">
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C94" t="s">
+      <c r="B94" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" t="s">
+      <c r="C94" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B95" t="s">
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C95" t="s">
+      <c r="B95" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96" t="s">
+      <c r="C95" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B96" t="s">
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C96" t="s">
+      <c r="B96" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" t="s">
+      <c r="C96" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B97" t="s">
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C97" t="s">
+      <c r="B97" s="1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
+      <c r="C97" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B98" t="s">
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C98" t="s">
+      <c r="B98" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" t="s">
+      <c r="C98" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B99" t="s">
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C99" t="s">
+      <c r="B99" s="1" t="s">
         <v>236</v>
       </c>
+      <c r="C99" s="1" t="s">
+        <v>237</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Shifted functions around and added comments
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -1077,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>